<commit_message>
đang dắt chỗ từ cũ bên controller study
</commit_message>
<xml_diff>
--- a/src/data/dataFile/xlsx/building dictionary.xlsx
+++ b/src/data/dataFile/xlsx/building dictionary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
   <si>
     <t>English</t>
   </si>
@@ -32,34 +32,37 @@
     <t>tây nguyên</t>
   </si>
   <si>
+    <t>easy</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>western europe</t>
+  </si>
+  <si>
+    <t>tây âu</t>
+  </si>
+  <si>
+    <t>western africa</t>
+  </si>
+  <si>
+    <t>tây phi</t>
+  </si>
+  <si>
+    <t>western asia</t>
+  </si>
+  <si>
+    <t>tây á</t>
+  </si>
+  <si>
+    <t>the mekong river delta</t>
+  </si>
+  <si>
+    <t>đồng bằng sông cửu long</t>
+  </si>
+  <si>
     <t>nothing</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>western europe</t>
-  </si>
-  <si>
-    <t>tây âu</t>
-  </si>
-  <si>
-    <t>western africa</t>
-  </si>
-  <si>
-    <t>tây phi</t>
-  </si>
-  <si>
-    <t>western asia</t>
-  </si>
-  <si>
-    <t>tây á</t>
-  </si>
-  <si>
-    <t>the mekong river delta</t>
-  </si>
-  <si>
-    <t>đồng bằng sông cửu long</t>
   </si>
   <si>
     <t>the northeast</t>
@@ -380,7 +383,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -388,13 +391,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -402,13 +405,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -416,13 +419,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -430,13 +433,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -444,13 +447,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -458,13 +461,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -472,13 +475,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -486,13 +489,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -500,13 +503,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -514,13 +517,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -528,13 +531,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -542,13 +545,13 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -556,13 +559,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -570,13 +573,13 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -584,13 +587,13 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -598,27 +601,27 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -626,13 +629,13 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -640,13 +643,13 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -654,13 +657,13 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -668,13 +671,13 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -682,13 +685,13 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -696,13 +699,13 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -710,13 +713,13 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -724,13 +727,13 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -738,27 +741,27 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -766,13 +769,13 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
@@ -780,13 +783,13 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -794,13 +797,13 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -808,13 +811,13 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Thêm xong tính năng ôn từ cũ
</commit_message>
<xml_diff>
--- a/src/data/dataFile/xlsx/building dictionary.xlsx
+++ b/src/data/dataFile/xlsx/building dictionary.xlsx
@@ -62,61 +62,61 @@
     <t>đồng bằng sông cửu long</t>
   </si>
   <si>
+    <t>the northeast</t>
+  </si>
+  <si>
+    <t>đông bắc</t>
+  </si>
+  <si>
+    <t>southern europe</t>
+  </si>
+  <si>
+    <t>nam âu</t>
+  </si>
+  <si>
+    <t>the north central coast</t>
+  </si>
+  <si>
+    <t>bắc trung bộ</t>
+  </si>
+  <si>
+    <t>north america</t>
+  </si>
+  <si>
+    <t>bắc mỹ</t>
+  </si>
+  <si>
+    <t>the south central coast</t>
+  </si>
+  <si>
+    <t>nam trung bộ</t>
+  </si>
+  <si>
+    <t>latin america</t>
+  </si>
+  <si>
+    <t>châu mỹ latin</t>
+  </si>
+  <si>
+    <t>northern africa</t>
+  </si>
+  <si>
+    <t>bắc phi</t>
+  </si>
+  <si>
+    <t>the red river delta</t>
+  </si>
+  <si>
+    <t>đồng bằng sông hồng</t>
+  </si>
+  <si>
+    <t>southeast asia</t>
+  </si>
+  <si>
+    <t>đông nam á</t>
+  </si>
+  <si>
     <t>nothing</t>
-  </si>
-  <si>
-    <t>the northeast</t>
-  </si>
-  <si>
-    <t>đông bắc</t>
-  </si>
-  <si>
-    <t>southern europe</t>
-  </si>
-  <si>
-    <t>nam âu</t>
-  </si>
-  <si>
-    <t>the north central coast</t>
-  </si>
-  <si>
-    <t>bắc trung bộ</t>
-  </si>
-  <si>
-    <t>north america</t>
-  </si>
-  <si>
-    <t>bắc mỹ</t>
-  </si>
-  <si>
-    <t>the south central coast</t>
-  </si>
-  <si>
-    <t>nam trung bộ</t>
-  </si>
-  <si>
-    <t>latin america</t>
-  </si>
-  <si>
-    <t>châu mỹ latin</t>
-  </si>
-  <si>
-    <t>northern africa</t>
-  </si>
-  <si>
-    <t>bắc phi</t>
-  </si>
-  <si>
-    <t>the red river delta</t>
-  </si>
-  <si>
-    <t>đồng bằng sông hồng</t>
-  </si>
-  <si>
-    <t>southeast asia</t>
-  </si>
-  <si>
-    <t>đông nam á</t>
   </si>
   <si>
     <t>europe</t>
@@ -383,7 +383,7 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -391,13 +391,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -405,13 +405,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
-        <v>20</v>
-      </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -419,13 +419,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
         <v>21</v>
       </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -433,13 +433,13 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
         <v>23</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -447,13 +447,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" t="s">
         <v>25</v>
       </c>
-      <c r="B11" t="s">
-        <v>26</v>
-      </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -461,13 +461,13 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="B12" t="s">
-        <v>28</v>
-      </c>
       <c r="C12" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
@@ -475,13 +475,13 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
@@ -489,13 +489,13 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
@@ -503,13 +503,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" t="s">
         <v>33</v>
       </c>
-      <c r="B15" t="s">
-        <v>34</v>
-      </c>
       <c r="C15" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -523,7 +523,7 @@
         <v>36</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -537,7 +537,7 @@
         <v>38</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -551,7 +551,7 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -565,7 +565,7 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -579,7 +579,7 @@
         <v>44</v>
       </c>
       <c r="C20" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -593,7 +593,7 @@
         <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -607,7 +607,7 @@
         <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D22" t="s">
         <v>49</v>
@@ -621,7 +621,7 @@
         <v>51</v>
       </c>
       <c r="C23" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -635,7 +635,7 @@
         <v>53</v>
       </c>
       <c r="C24" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -649,7 +649,7 @@
         <v>55</v>
       </c>
       <c r="C25" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -663,7 +663,7 @@
         <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -677,7 +677,7 @@
         <v>59</v>
       </c>
       <c r="C27" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -691,7 +691,7 @@
         <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -705,7 +705,7 @@
         <v>63</v>
       </c>
       <c r="C29" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -719,7 +719,7 @@
         <v>65</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -733,7 +733,7 @@
         <v>67</v>
       </c>
       <c r="C31" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -747,7 +747,7 @@
         <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
         <v>70</v>
@@ -761,7 +761,7 @@
         <v>72</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -775,7 +775,7 @@
         <v>74</v>
       </c>
       <c r="C34" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
@@ -789,7 +789,7 @@
         <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -803,7 +803,7 @@
         <v>78</v>
       </c>
       <c r="C36" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -817,7 +817,7 @@
         <v>80</v>
       </c>
       <c r="C37" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Design xong 2 cái nút ở Home
</commit_message>
<xml_diff>
--- a/src/data/dataFile/xlsx/building dictionary.xlsx
+++ b/src/data/dataFile/xlsx/building dictionary.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="82">
   <si>
     <t>English</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>tây bắc</t>
+  </si>
+  <si>
+    <t>moderate</t>
   </si>
   <si>
     <t>middle africa</t>
@@ -551,7 +554,7 @@
         <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
@@ -565,7 +568,7 @@
         <v>42</v>
       </c>
       <c r="C19" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -573,10 +576,10 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C20" t="s">
         <v>34</v>
@@ -587,10 +590,10 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C21" t="s">
         <v>34</v>
@@ -601,24 +604,24 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C22" t="s">
         <v>34</v>
       </c>
       <c r="D22" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C23" t="s">
         <v>34</v>
@@ -629,10 +632,10 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
@@ -643,10 +646,10 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
         <v>34</v>
@@ -657,10 +660,10 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
@@ -671,10 +674,10 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C27" t="s">
         <v>34</v>
@@ -685,10 +688,10 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
         <v>34</v>
@@ -699,10 +702,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B29" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
@@ -713,10 +716,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C30" t="s">
         <v>34</v>
@@ -727,10 +730,10 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C31" t="s">
         <v>34</v>
@@ -741,24 +744,24 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C32" t="s">
         <v>34</v>
       </c>
       <c r="D32" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B33" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C33" t="s">
         <v>34</v>
@@ -769,10 +772,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
@@ -783,10 +786,10 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B35" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C35" t="s">
         <v>34</v>
@@ -797,10 +800,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B36" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C36" t="s">
         <v>34</v>
@@ -811,10 +814,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C37" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
Chắc ko thêm gì nữa
</commit_message>
<xml_diff>
--- a/src/data/dataFile/xlsx/building dictionary.xlsx
+++ b/src/data/dataFile/xlsx/building dictionary.xlsx
@@ -44,6 +44,9 @@
     <t>tây âu</t>
   </si>
   <si>
+    <t>moderate</t>
+  </si>
+  <si>
     <t>western africa</t>
   </si>
   <si>
@@ -141,9 +144,6 @@
   </si>
   <si>
     <t>tây bắc</t>
-  </si>
-  <si>
-    <t>moderate</t>
   </si>
   <si>
     <t>middle africa</t>
@@ -344,7 +344,7 @@
         <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -352,13 +352,13 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -366,13 +366,13 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -380,10 +380,10 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -394,13 +394,13 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -408,13 +408,13 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>7</v>
@@ -422,13 +422,13 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -436,10 +436,10 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
@@ -450,13 +450,13 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
@@ -464,10 +464,10 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -478,10 +478,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
         <v>6</v>
@@ -492,10 +492,10 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -506,13 +506,13 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
@@ -520,13 +520,13 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
@@ -534,13 +534,13 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
@@ -548,10 +548,10 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C18" t="s">
         <v>6</v>
@@ -562,13 +562,13 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
@@ -582,7 +582,7 @@
         <v>45</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
@@ -596,7 +596,7 @@
         <v>47</v>
       </c>
       <c r="C21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
@@ -610,7 +610,7 @@
         <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
         <v>50</v>
@@ -624,7 +624,7 @@
         <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D23" t="s">
         <v>7</v>
@@ -638,7 +638,7 @@
         <v>54</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D24" t="s">
         <v>7</v>
@@ -652,7 +652,7 @@
         <v>56</v>
       </c>
       <c r="C25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
@@ -666,7 +666,7 @@
         <v>58</v>
       </c>
       <c r="C26" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
@@ -680,7 +680,7 @@
         <v>60</v>
       </c>
       <c r="C27" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
@@ -694,7 +694,7 @@
         <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
@@ -708,7 +708,7 @@
         <v>64</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
@@ -722,7 +722,7 @@
         <v>66</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
@@ -736,7 +736,7 @@
         <v>68</v>
       </c>
       <c r="C31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
@@ -750,7 +750,7 @@
         <v>70</v>
       </c>
       <c r="C32" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D32" t="s">
         <v>71</v>
@@ -764,7 +764,7 @@
         <v>73</v>
       </c>
       <c r="C33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -778,7 +778,7 @@
         <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D34" t="s">
         <v>7</v>
@@ -792,7 +792,7 @@
         <v>77</v>
       </c>
       <c r="C35" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D35" t="s">
         <v>7</v>
@@ -806,7 +806,7 @@
         <v>79</v>
       </c>
       <c r="C36" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D36" t="s">
         <v>7</v>
@@ -820,7 +820,7 @@
         <v>81</v>
       </c>
       <c r="C37" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D37" t="s">
         <v>7</v>

</xml_diff>